<commit_message>
Upload SNA example. Modify grade names
</commit_message>
<xml_diff>
--- a/1_moodleLAcourse/Results.xlsx
+++ b/1_moodleLAcourse/Results.xlsx
@@ -17,43 +17,43 @@
     <t xml:space="preserve">user</t>
   </si>
   <si>
-    <t xml:space="preserve">SNA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNA_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group_self</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group_All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Excercises</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Literature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Theory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ethics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Critique</t>
+    <t xml:space="preserve">Grade.SNA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade.SNA_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade.Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade.Group_self</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade.Group_All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade.Excercises</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade.Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade.Literature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade.Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade.Introduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade.Theory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade.Ethics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade.Critique</t>
   </si>
   <si>
     <t xml:space="preserve">Final_grade</t>

</xml_diff>